<commit_message>
Added respond to a foreclosure to spreadsheet list
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AEE42B-87F1-4971-ADF0-DA16C59E9A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23EEBFB-E4DB-43CE-832B-8E14A9833B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="264" windowWidth="23016" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>name</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/financial-affidavit</t>
+  </si>
+  <si>
+    <t>Respond to a mortgage foreclosure complaint</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/respond-mortgage-foreclosure-complaint</t>
   </si>
 </sst>
 </file>
@@ -627,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -897,65 +903,73 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -969,18 +983,18 @@
     <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="B12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B35" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B36" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B38" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B39" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B31" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="B9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="B32" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B40" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B41" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="B18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B39" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B40" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="B27" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="B28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="B26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
@@ -989,11 +1003,11 @@
     <hyperlink ref="B21" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B5" r:id="rId24" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
     <hyperlink ref="B11" r:id="rId25" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B36" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B37" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
     <hyperlink ref="B30" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B33" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B37" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B34" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B34" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B38" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B35" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
     <hyperlink ref="B7" r:id="rId31" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
     <hyperlink ref="B16" r:id="rId32" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Added SNCO to easy forms list spreadsheet
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23EEBFB-E4DB-43CE-832B-8E14A9833B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB29350D-D5F7-46A1-A7C2-E0958C908BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>name</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/respond-mortgage-foreclosure-complaint</t>
+  </si>
+  <si>
+    <t>Stalking No Contact Order - SNCO</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/stalking-no-contact-order-request</t>
   </si>
 </sst>
 </file>
@@ -633,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,25 +957,33 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -985,16 +999,16 @@
     <hyperlink ref="B12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="B36" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B39" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B40" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B31" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="B9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="B32" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B41" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B42" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="B18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B40" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B41" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="B27" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="B28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="B26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>

</xml_diff>

<commit_message>
updated easy form list added custom email forms to self button text
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB29350D-D5F7-46A1-A7C2-E0958C908BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F817BF-5F5F-4278-9156-56CF0EB3C05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>name</t>
   </si>
@@ -277,6 +277,24 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/stalking-no-contact-order-request</t>
+  </si>
+  <si>
+    <t>Vacate a default judgment within 30 days</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/special-process-server-request</t>
+  </si>
+  <si>
+    <t>Request to approve an unlicensed process server</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/vacate-default-judgment-within-30-days</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/motion-continue-or-extend-time</t>
+  </si>
+  <si>
+    <t>Motion to continue or extend time</t>
   </si>
 </sst>
 </file>
@@ -639,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,177 +831,201 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -997,33 +1039,36 @@
     <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="B12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B36" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B38" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B40" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B31" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B42" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B32" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="B9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B32" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B42" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B34" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B45" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="B18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B41" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B27" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B23" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B21" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B43" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B28" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B29" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B27" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B26" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B22" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B5" r:id="rId24" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
     <hyperlink ref="B11" r:id="rId25" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B37" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
-    <hyperlink ref="B30" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B34" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B38" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B35" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B39" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B31" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
+    <hyperlink ref="B36" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B40" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B37" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
     <hyperlink ref="B7" r:id="rId31" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
     <hyperlink ref="B16" r:id="rId32" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
+    <hyperlink ref="B33" r:id="rId33" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
+    <hyperlink ref="B44" r:id="rId34" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
+    <hyperlink ref="B21" r:id="rId35" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated ilao easy form list - vessa letter title
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F817BF-5F5F-4278-9156-56CF0EB3C05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C08D10-3947-46E6-9B14-44287D9F3557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34860" yWindow="-2985" windowWidth="27015" windowHeight="17430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>https://www.illinoislegalaid.org/legal-information/stop-wage-assignment-letter</t>
   </si>
   <si>
-    <t>Request time off work due to domestic violence</t>
-  </si>
-  <si>
     <t>https://www.illinoislegalaid.org/legal-information/request-time-work-due-domestic-abuse-letter</t>
   </si>
   <si>
@@ -295,6 +292,9 @@
   </si>
   <si>
     <t>Motion to continue or extend time</t>
+  </si>
+  <si>
+    <t>Request time off work due after surviving violence</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,10 +687,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -703,10 +703,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -719,42 +719,42 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -775,10 +775,10 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -791,10 +791,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -807,162 +807,162 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -975,26 +975,26 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1007,26 +1007,26 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added divorce and parenting plan to xlsx
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C08D10-3947-46E6-9B14-44287D9F3557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521BA7F2-7530-49B6-ACD1-C49D6F5DA128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34860" yWindow="-2985" windowWidth="27015" windowHeight="17430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>name</t>
   </si>
@@ -295,6 +295,18 @@
   </si>
   <si>
     <t>Request time off work due after surviving violence</t>
+  </si>
+  <si>
+    <t>Divorce</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/divorce</t>
+  </si>
+  <si>
+    <t>Parenting plan</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/parenting-plan</t>
   </si>
 </sst>
 </file>
@@ -657,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,348 +739,364 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
-    <sortCondition ref="A2:A15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
+    <sortCondition ref="A2:A16"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B38" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B42" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B32" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B34" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B45" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B43" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B28" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B29" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B27" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B26" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B24" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B22" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B40" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B18" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B44" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B34" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B11" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B36" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B47" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B45" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B31" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B29" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B28" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B25" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B23" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B5" r:id="rId24" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
-    <hyperlink ref="B11" r:id="rId25" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B39" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
-    <hyperlink ref="B31" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B36" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B40" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B37" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B12" r:id="rId25" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
+    <hyperlink ref="B41" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B33" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
+    <hyperlink ref="B38" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B42" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B39" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
     <hyperlink ref="B7" r:id="rId31" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
-    <hyperlink ref="B16" r:id="rId32" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
-    <hyperlink ref="B33" r:id="rId33" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
-    <hyperlink ref="B44" r:id="rId34" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
-    <hyperlink ref="B21" r:id="rId35" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
+    <hyperlink ref="B17" r:id="rId32" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
+    <hyperlink ref="B35" r:id="rId33" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
+    <hyperlink ref="B46" r:id="rId34" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
+    <hyperlink ref="B22" r:id="rId35" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Delay a Foreclosure Sale to spreadsheet file
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521BA7F2-7530-49B6-ACD1-C49D6F5DA128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F6B699-F12C-4D6B-AFBB-9B29353C1E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>name</t>
   </si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/parenting-plan</t>
+  </si>
+  <si>
+    <t>Delay a foreclosure sale</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/delay-foreclosure-sale</t>
   </si>
 </sst>
 </file>
@@ -669,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,364 +745,372 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
-    <sortCondition ref="A2:A16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
+    <sortCondition ref="A2:A17"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B40" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B18" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B44" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B34" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B11" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B36" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B47" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B45" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B31" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B29" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B28" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B25" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B23" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B14" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B41" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B19" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B45" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B35" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B37" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B48" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B20" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B22" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B46" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B31" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B32" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B30" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B29" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B26" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B5" r:id="rId24" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
-    <hyperlink ref="B12" r:id="rId25" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B41" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
-    <hyperlink ref="B33" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B38" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B42" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B39" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B13" r:id="rId25" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
+    <hyperlink ref="B42" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B34" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
+    <hyperlink ref="B39" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B43" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B40" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
     <hyperlink ref="B7" r:id="rId31" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
-    <hyperlink ref="B17" r:id="rId32" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
-    <hyperlink ref="B35" r:id="rId33" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
-    <hyperlink ref="B46" r:id="rId34" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
-    <hyperlink ref="B22" r:id="rId35" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
+    <hyperlink ref="B18" r:id="rId32" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
+    <hyperlink ref="B36" r:id="rId33" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
+    <hyperlink ref="B47" r:id="rId34" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
+    <hyperlink ref="B23" r:id="rId35" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added debt collector letter to xlsx
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F6B699-F12C-4D6B-AFBB-9B29353C1E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7463C910-0A35-48AC-A67A-813D3383FCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33345" yWindow="-3150" windowWidth="23790" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>name</t>
   </si>
@@ -48,18 +48,6 @@
     <t>https://www.illinoislegalaid.org/legal-information/fee-waiver</t>
   </si>
   <si>
-    <t>Collection proof letter</t>
-  </si>
-  <si>
-    <t>https://www.illinoislegalaid.org/legal-information/collection-proof-debtor-letter</t>
-  </si>
-  <si>
-    <t>Ask debt collector to stop contact</t>
-  </si>
-  <si>
-    <t>https://www.illinoislegalaid.org/legal-information/request-collection-agency-stop-contacting</t>
-  </si>
-  <si>
     <t>https://www.illinoislegalaid.org/legal-information/end-illegal-lockout-demand</t>
   </si>
   <si>
@@ -313,6 +301,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/delay-foreclosure-sale</t>
+  </si>
+  <si>
+    <t>Debt collector letter</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/debt-collector-letter</t>
   </si>
 </sst>
 </file>
@@ -675,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,412 +699,403 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
-    <sortCondition ref="A2:A17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
+    <sortCondition ref="A2:A16"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B14" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B41" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B19" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B45" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B35" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B37" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B48" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B20" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B22" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B46" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B31" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B32" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B30" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B29" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B26" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B24" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
-    <hyperlink ref="B5" r:id="rId24" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
-    <hyperlink ref="B13" r:id="rId25" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B42" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
-    <hyperlink ref="B34" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B39" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B43" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B40" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
-    <hyperlink ref="B7" r:id="rId31" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
-    <hyperlink ref="B18" r:id="rId32" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
-    <hyperlink ref="B36" r:id="rId33" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
-    <hyperlink ref="B47" r:id="rId34" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
-    <hyperlink ref="B23" r:id="rId35" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
+    <hyperlink ref="B16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B40" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B18" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B44" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B34" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B36" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B47" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B21" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B45" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B30" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B31" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B29" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B25" r:id="rId20" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B4" r:id="rId22" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
+    <hyperlink ref="B12" r:id="rId23" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
+    <hyperlink ref="B41" r:id="rId24" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B33" r:id="rId25" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
+    <hyperlink ref="B38" r:id="rId26" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B42" r:id="rId27" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B39" r:id="rId28" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B5" r:id="rId29" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
+    <hyperlink ref="B17" r:id="rId30" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
+    <hyperlink ref="B35" r:id="rId31" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
+    <hyperlink ref="B46" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
+    <hyperlink ref="B22" r:id="rId33" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
+    <hyperlink ref="B6" r:id="rId34" xr:uid="{A79B08AB-EC87-4B3E-B1A5-DB2982598670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added CNCO to easy form spreadsheet
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7463C910-0A35-48AC-A67A-813D3383FCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E448E05-29D1-4219-95E5-208B78122B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33345" yWindow="-3150" windowWidth="23790" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>name</t>
   </si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/debt-collector-letter</t>
+  </si>
+  <si>
+    <t>Civil No Contact Order - CNCO</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/civil-no-contact-order-request</t>
   </si>
 </sst>
 </file>
@@ -669,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,387 +721,395 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
-    <sortCondition ref="A2:A16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
+    <sortCondition ref="A2:A17"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B40" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B18" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B44" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B34" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B36" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B47" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B21" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B45" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B30" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B31" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B29" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B25" r:id="rId20" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B23" r:id="rId21" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B41" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B19" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B45" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B35" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B48" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B20" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B46" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B31" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B32" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B29" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B26" r:id="rId20" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B24" r:id="rId21" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B4" r:id="rId22" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
-    <hyperlink ref="B12" r:id="rId23" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B41" r:id="rId24" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
-    <hyperlink ref="B33" r:id="rId25" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B38" r:id="rId26" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B42" r:id="rId27" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B39" r:id="rId28" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
-    <hyperlink ref="B5" r:id="rId29" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
-    <hyperlink ref="B17" r:id="rId30" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
-    <hyperlink ref="B35" r:id="rId31" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
-    <hyperlink ref="B46" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
-    <hyperlink ref="B22" r:id="rId33" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
-    <hyperlink ref="B6" r:id="rId34" xr:uid="{A79B08AB-EC87-4B3E-B1A5-DB2982598670}"/>
+    <hyperlink ref="B13" r:id="rId23" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
+    <hyperlink ref="B42" r:id="rId24" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B34" r:id="rId25" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
+    <hyperlink ref="B39" r:id="rId26" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B43" r:id="rId27" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B40" r:id="rId28" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B6" r:id="rId29" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
+    <hyperlink ref="B18" r:id="rId30" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
+    <hyperlink ref="B36" r:id="rId31" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
+    <hyperlink ref="B47" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
+    <hyperlink ref="B23" r:id="rId33" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
+    <hyperlink ref="B7" r:id="rId34" xr:uid="{A79B08AB-EC87-4B3E-B1A5-DB2982598670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated xlsx default_home and interview_list
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E448E05-29D1-4219-95E5-208B78122B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69CFA8D-8C6D-4EC2-9395-457A388BAEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5340" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>name</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/civil-no-contact-order-request</t>
+  </si>
+  <si>
+    <t>Citation to discover assets to debtor</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/citation-discover-assets-debtor</t>
   </si>
 </sst>
 </file>
@@ -675,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,395 +727,403 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
-    <sortCondition ref="A2:A17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B18">
+    <sortCondition ref="A2:A18"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B41" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B19" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B45" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B35" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B48" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B20" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B46" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B31" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B32" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B29" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B26" r:id="rId20" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B24" r:id="rId21" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B42" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B20" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B46" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B36" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B38" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B49" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B47" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B32" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B33" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B31" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B30" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B27" r:id="rId20" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B4" r:id="rId22" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
-    <hyperlink ref="B13" r:id="rId23" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B42" r:id="rId24" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
-    <hyperlink ref="B34" r:id="rId25" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B39" r:id="rId26" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B43" r:id="rId27" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B40" r:id="rId28" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
-    <hyperlink ref="B6" r:id="rId29" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
-    <hyperlink ref="B18" r:id="rId30" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
-    <hyperlink ref="B36" r:id="rId31" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
-    <hyperlink ref="B47" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
-    <hyperlink ref="B23" r:id="rId33" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
-    <hyperlink ref="B7" r:id="rId34" xr:uid="{A79B08AB-EC87-4B3E-B1A5-DB2982598670}"/>
+    <hyperlink ref="B14" r:id="rId23" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
+    <hyperlink ref="B43" r:id="rId24" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B35" r:id="rId25" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
+    <hyperlink ref="B40" r:id="rId26" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B44" r:id="rId27" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B41" r:id="rId28" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B7" r:id="rId29" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
+    <hyperlink ref="B19" r:id="rId30" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
+    <hyperlink ref="B37" r:id="rId31" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
+    <hyperlink ref="B48" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
+    <hyperlink ref="B24" r:id="rId33" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
+    <hyperlink ref="B8" r:id="rId34" xr:uid="{A79B08AB-EC87-4B3E-B1A5-DB2982598670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added child support mod to xlsx
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2289579-F4E3-4816-8E33-85C66AD7479E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020E4919-2A22-42D0-A769-398D190EFE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33525" yWindow="-2955" windowWidth="23010" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5340" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>name</t>
   </si>
@@ -325,6 +325,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/unemployment-benefits-request-hearing</t>
+  </si>
+  <si>
+    <t>Request to change child support</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/child-support-modification</t>
   </si>
 </sst>
 </file>
@@ -687,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,105 +1003,113 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1107,18 +1121,18 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B42" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B43" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B20" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B46" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B47" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B36" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="B12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B38" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B50" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B39" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B51" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="B21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="B23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B47" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B48" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="B32" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="B33" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="B31" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
@@ -1127,18 +1141,19 @@
     <hyperlink ref="B25" r:id="rId21" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B4" r:id="rId22" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
     <hyperlink ref="B14" r:id="rId23" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B43" r:id="rId24" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B44" r:id="rId24" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
     <hyperlink ref="B35" r:id="rId25" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B40" r:id="rId26" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B44" r:id="rId27" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B41" r:id="rId28" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B41" r:id="rId26" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B45" r:id="rId27" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B42" r:id="rId28" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
     <hyperlink ref="B7" r:id="rId29" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
     <hyperlink ref="B19" r:id="rId30" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
     <hyperlink ref="B37" r:id="rId31" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
-    <hyperlink ref="B49" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
+    <hyperlink ref="B50" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
     <hyperlink ref="B24" r:id="rId33" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
     <hyperlink ref="B8" r:id="rId34" xr:uid="{A79B08AB-EC87-4B3E-B1A5-DB2982598670}"/>
-    <hyperlink ref="B48" r:id="rId35" xr:uid="{ACF5336B-7760-4E17-AB95-B490DF08E9B7}"/>
+    <hyperlink ref="B49" r:id="rId35" xr:uid="{ACF5336B-7760-4E17-AB95-B490DF08E9B7}"/>
+    <hyperlink ref="B38" r:id="rId36" xr:uid="{5B5F40DA-F64F-4CBD-A95F-EBC3267FFA16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated easy form xlsx and reverted error message code while troubleshooting
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020E4919-2A22-42D0-A769-398D190EFE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF4FF14-710D-4455-958E-00F8B54567FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5340" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -282,9 +282,6 @@
     <t>Motion to continue or extend time</t>
   </si>
   <si>
-    <t>Request time off work due after surviving violence</t>
-  </si>
-  <si>
     <t>Divorce</t>
   </si>
   <si>
@@ -331,6 +328,9 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/child-support-modification</t>
+  </si>
+  <si>
+    <t>Request time off work  after surviving violence</t>
   </si>
 </sst>
 </file>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,18 +739,18 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -763,26 +763,26 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -923,10 +923,10 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -987,7 +987,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>16</v>
@@ -1003,10 +1003,10 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1091,10 +1091,10 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Vacate default foreclosure
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Desktop\Easy Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF4FF14-710D-4455-958E-00F8B54567FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A34298-DF6E-44B5-BD68-5C2932D3090D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>name</t>
   </si>
@@ -331,6 +331,12 @@
   </si>
   <si>
     <t>Request time off work  after surviving violence</t>
+  </si>
+  <si>
+    <t>Vacate a default judgment of foreclosure</t>
+  </si>
+  <si>
+    <t>https://easyforms.illinoislegalaid.org/start/VacateDefaultForeclosure/vacate_default_foreclosure</t>
   </si>
 </sst>
 </file>
@@ -693,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1099,17 +1105,25 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1129,7 +1143,7 @@
     <hyperlink ref="B12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="B39" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B51" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B52" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="B21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="B23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="B48" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
@@ -1149,11 +1163,12 @@
     <hyperlink ref="B7" r:id="rId29" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
     <hyperlink ref="B19" r:id="rId30" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
     <hyperlink ref="B37" r:id="rId31" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
-    <hyperlink ref="B50" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
+    <hyperlink ref="B51" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
     <hyperlink ref="B24" r:id="rId33" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
     <hyperlink ref="B8" r:id="rId34" xr:uid="{A79B08AB-EC87-4B3E-B1A5-DB2982598670}"/>
     <hyperlink ref="B49" r:id="rId35" xr:uid="{ACF5336B-7760-4E17-AB95-B490DF08E9B7}"/>
     <hyperlink ref="B38" r:id="rId36" xr:uid="{5B5F40DA-F64F-4CBD-A95F-EBC3267FFA16}"/>
+    <hyperlink ref="B50" r:id="rId37" xr:uid="{CE808D58-61B9-423B-AD81-E68A94792CFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Emergency Motion to Claim Exemption to spreadsheet
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Desktop\Easy Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A34298-DF6E-44B5-BD68-5C2932D3090D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC00570-497F-4684-9839-952ABB0759D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>name</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>https://easyforms.illinoislegalaid.org/start/VacateDefaultForeclosure/vacate_default_foreclosure</t>
+  </si>
+  <si>
+    <t>Emergency Motion to Claim Exemption</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/emergency-motion-claim-exemption</t>
   </si>
 </sst>
 </file>
@@ -699,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,358 +823,366 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>29</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B18">
-    <sortCondition ref="A2:A18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B19">
+    <sortCondition ref="A2:A19"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B43" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B20" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B47" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B36" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B16" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B44" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B21" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B48" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B37" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="B12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B39" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B52" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B48" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B32" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B33" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B31" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B30" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B27" r:id="rId20" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B25" r:id="rId21" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B40" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B53" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B22" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B24" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B49" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B33" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B34" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B32" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B31" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B28" r:id="rId20" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B26" r:id="rId21" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B4" r:id="rId22" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
-    <hyperlink ref="B14" r:id="rId23" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B44" r:id="rId24" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
-    <hyperlink ref="B35" r:id="rId25" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B41" r:id="rId26" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B45" r:id="rId27" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B42" r:id="rId28" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B15" r:id="rId23" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
+    <hyperlink ref="B45" r:id="rId24" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B36" r:id="rId25" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
+    <hyperlink ref="B42" r:id="rId26" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B46" r:id="rId27" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B43" r:id="rId28" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
     <hyperlink ref="B7" r:id="rId29" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
-    <hyperlink ref="B19" r:id="rId30" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
-    <hyperlink ref="B37" r:id="rId31" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
-    <hyperlink ref="B51" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
-    <hyperlink ref="B24" r:id="rId33" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
+    <hyperlink ref="B20" r:id="rId30" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
+    <hyperlink ref="B38" r:id="rId31" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
+    <hyperlink ref="B52" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
+    <hyperlink ref="B25" r:id="rId33" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
     <hyperlink ref="B8" r:id="rId34" xr:uid="{A79B08AB-EC87-4B3E-B1A5-DB2982598670}"/>
-    <hyperlink ref="B49" r:id="rId35" xr:uid="{ACF5336B-7760-4E17-AB95-B490DF08E9B7}"/>
-    <hyperlink ref="B38" r:id="rId36" xr:uid="{5B5F40DA-F64F-4CBD-A95F-EBC3267FFA16}"/>
-    <hyperlink ref="B50" r:id="rId37" xr:uid="{CE808D58-61B9-423B-AD81-E68A94792CFB}"/>
+    <hyperlink ref="B50" r:id="rId35" xr:uid="{ACF5336B-7760-4E17-AB95-B490DF08E9B7}"/>
+    <hyperlink ref="B39" r:id="rId36" xr:uid="{5B5F40DA-F64F-4CBD-A95F-EBC3267FFA16}"/>
+    <hyperlink ref="B51" r:id="rId37" xr:uid="{CE808D58-61B9-423B-AD81-E68A94792CFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added joint simplified divorce to xlsx
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Desktop\Easy Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC00570-497F-4684-9839-952ABB0759D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC40A0F1-FAD3-4FF9-B622-655BE620B087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34425" yWindow="-2655" windowWidth="30840" windowHeight="17085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>name</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/emergency-motion-claim-exemption</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/joint-simplified-divorce-cook-county</t>
+  </si>
+  <si>
+    <t>Joint simplified divorce - Cook County</t>
   </si>
 </sst>
 </file>
@@ -705,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,249 +901,257 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>107</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1149,40 +1163,41 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B16" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B44" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B45" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B21" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B48" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B37" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B49" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B38" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="B12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B40" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B53" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B41" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B54" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="B22" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B24" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B49" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B33" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B34" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B32" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B31" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B28" r:id="rId20" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B26" r:id="rId21" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B25" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B50" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B34" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B35" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B33" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B32" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B29" r:id="rId20" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B27" r:id="rId21" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B4" r:id="rId22" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
     <hyperlink ref="B15" r:id="rId23" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B45" r:id="rId24" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
-    <hyperlink ref="B36" r:id="rId25" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B42" r:id="rId26" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B46" r:id="rId27" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B43" r:id="rId28" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B46" r:id="rId24" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B37" r:id="rId25" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
+    <hyperlink ref="B43" r:id="rId26" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B47" r:id="rId27" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B44" r:id="rId28" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
     <hyperlink ref="B7" r:id="rId29" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
     <hyperlink ref="B20" r:id="rId30" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
-    <hyperlink ref="B38" r:id="rId31" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
-    <hyperlink ref="B52" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
-    <hyperlink ref="B25" r:id="rId33" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
+    <hyperlink ref="B39" r:id="rId31" xr:uid="{7A05A07A-CD46-49E0-8CAA-F7A2359DAFA6}"/>
+    <hyperlink ref="B53" r:id="rId32" xr:uid="{E8243C89-C7E6-4F98-8AB2-6F1F40304356}"/>
+    <hyperlink ref="B26" r:id="rId33" xr:uid="{A702F17D-AC4F-43CE-B44D-BF0EB0BA16F4}"/>
     <hyperlink ref="B8" r:id="rId34" xr:uid="{A79B08AB-EC87-4B3E-B1A5-DB2982598670}"/>
-    <hyperlink ref="B50" r:id="rId35" xr:uid="{ACF5336B-7760-4E17-AB95-B490DF08E9B7}"/>
-    <hyperlink ref="B39" r:id="rId36" xr:uid="{5B5F40DA-F64F-4CBD-A95F-EBC3267FFA16}"/>
-    <hyperlink ref="B51" r:id="rId37" xr:uid="{CE808D58-61B9-423B-AD81-E68A94792CFB}"/>
+    <hyperlink ref="B51" r:id="rId35" xr:uid="{ACF5336B-7760-4E17-AB95-B490DF08E9B7}"/>
+    <hyperlink ref="B40" r:id="rId36" xr:uid="{5B5F40DA-F64F-4CBD-A95F-EBC3267FFA16}"/>
+    <hyperlink ref="B52" r:id="rId37" xr:uid="{CE808D58-61B9-423B-AD81-E68A94792CFB}"/>
+    <hyperlink ref="B23" r:id="rId38" xr:uid="{F1297A01-61E3-4759-9D5D-D9A6F9BCB77E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated VAP program name
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC40A0F1-FAD3-4FF9-B622-655BE620B087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88F28DB-BA70-47F2-B161-683459368F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34425" yWindow="-2655" windowWidth="30840" windowHeight="17085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>https://www.illinoislegalaid.org/legal-information/respond-lawsuit</t>
   </si>
   <si>
-    <t>Voluntary acknowledgment of paternity - VAP</t>
-  </si>
-  <si>
     <t>https://www.illinoislegalaid.org/legal-information/voluntary-acknowledgment-parentage-vap</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>Joint simplified divorce - Cook County</t>
+  </si>
+  <si>
+    <t>Voluntary acknowledgment of parentage - VAP</t>
   </si>
 </sst>
 </file>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,58 +749,58 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -829,18 +829,18 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -861,10 +861,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -877,10 +877,10 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -893,18 +893,18 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -917,111 +917,111 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>16</v>
@@ -1029,18 +1029,18 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1053,26 +1053,26 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1085,26 +1085,26 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1117,42 +1117,42 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>